<commit_message>
got some html contents
</commit_message>
<xml_diff>
--- a/temp/study material.xlsx
+++ b/temp/study material.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91949\Desktop\uneducated-coder\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0844B0-4ADE-40A6-8536-C852CE38A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4E5C1E-D692-426E-AF88-B815F94CCA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="JS" sheetId="1" r:id="rId1"/>
-    <sheet name="DSA" sheetId="8" r:id="rId2"/>
-    <sheet name="Node" sheetId="2" r:id="rId3"/>
-    <sheet name="Node GIT" sheetId="9" r:id="rId4"/>
-    <sheet name="MongoDB" sheetId="3" r:id="rId5"/>
-    <sheet name="common DB" sheetId="4" r:id="rId6"/>
-    <sheet name="express" sheetId="5" r:id="rId7"/>
-    <sheet name="Computer science" sheetId="7" r:id="rId8"/>
-    <sheet name="React" sheetId="6" r:id="rId9"/>
+    <sheet name="HTML" sheetId="10" r:id="rId1"/>
+    <sheet name="CSS" sheetId="11" r:id="rId2"/>
+    <sheet name="JS" sheetId="1" r:id="rId3"/>
+    <sheet name="DSA" sheetId="8" r:id="rId4"/>
+    <sheet name="Node" sheetId="2" r:id="rId5"/>
+    <sheet name="Node GIT" sheetId="9" r:id="rId6"/>
+    <sheet name="MongoDB" sheetId="3" r:id="rId7"/>
+    <sheet name="common DB" sheetId="4" r:id="rId8"/>
+    <sheet name="express" sheetId="5" r:id="rId9"/>
+    <sheet name="Computer science" sheetId="7" r:id="rId10"/>
+    <sheet name="React" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>What is Javascript</t>
   </si>
@@ -374,6 +376,15 @@
   </si>
   <si>
     <t>REPL</t>
+  </si>
+  <si>
+    <t>What is HTML?</t>
+  </si>
+  <si>
+    <t>What is Markup language?</t>
+  </si>
+  <si>
+    <t>HTML vs HTML5</t>
   </si>
 </sst>
 </file>
@@ -712,66 +723,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E22862-179B-4147-A3BF-4A6DE02934C2}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="2" width="45.21875" customWidth="1"/>
-    <col min="3" max="3" width="69.77734375" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" customWidth="1"/>
+    <col min="2" max="2" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -779,316 +754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA2F53F-3B2D-4061-A513-BAC0D67090E3}">
-  <dimension ref="A16:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D77997-2DA0-42EF-9E5C-889A7E65CAAA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="63.33203125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0E838A-79DB-4648-BF84-239CF84E8B43}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="77.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE6F591-F378-4794-8EC5-154CA394494A}">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90D9F36-2DF1-4026-BBDF-7BB25E3656DE}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="51.6640625" customWidth="1"/>
-    <col min="2" max="2" width="61.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9239E2BD-23D4-4F29-A572-03C4CC080FD6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D642969-0CAE-499D-9E50-3C8C1AB1B467}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -1302,7 +968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5E2BBA-BFCB-48C0-A46F-42B9AF3F662A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1350,4 +1016,395 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF84ED45-F8BA-44AA-BA33-2EAF018F4B36}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" customWidth="1"/>
+    <col min="3" max="3" width="69.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA2F53F-3B2D-4061-A513-BAC0D67090E3}">
+  <dimension ref="A16:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="70.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D77997-2DA0-42EF-9E5C-889A7E65CAAA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="63.33203125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0E838A-79DB-4648-BF84-239CF84E8B43}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="77.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE6F591-F378-4794-8EC5-154CA394494A}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90D9F36-2DF1-4026-BBDF-7BB25E3656DE}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9239E2BD-23D4-4F29-A572-03C4CC080FD6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>